<commit_message>
implementacion tabla habilidad en excel y workbench mas foto
</commit_message>
<xml_diff>
--- a/dojos_y_ninjas.xlsx
+++ b/dojos_y_ninjas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\Desktop\apuntesPython\apuntesClase\SQL\06_erd-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF781CE-F818-452A-B2F4-A3DD02B09BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E624C834-EE81-44A0-82A6-57C58EC25A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{96022472-ABAC-4D18-BB59-4F185A56C18E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>dojo</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>karate</t>
+  </si>
+  <si>
+    <t>id_habilidad</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB1D070-0521-48AA-8BCB-E4ED56EE80DA}">
-  <dimension ref="B3:M6"/>
+  <dimension ref="B3:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
         <v>8</v>
@@ -497,8 +500,8 @@
       <c r="K5" t="s">
         <v>12</v>
       </c>
-      <c r="L5" t="s">
-        <v>13</v>
+      <c r="L5">
+        <v>1</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -516,6 +519,27 @@
       </c>
       <c r="J6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ejercicio blog y dashboard
</commit_message>
<xml_diff>
--- a/dojos_y_ninjas.xlsx
+++ b/dojos_y_ninjas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\Desktop\apuntesPython\apuntesClase\SQL\06_erd-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E624C834-EE81-44A0-82A6-57C58EC25A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A0E4AA-274A-44E4-819A-603FF7E64FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{96022472-ABAC-4D18-BB59-4F185A56C18E}"/>
   </bookViews>
@@ -25,26 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
-  <si>
-    <t>dojo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>ubicación</t>
-  </si>
-  <si>
     <t>calle</t>
   </si>
   <si>
     <t>numero</t>
   </si>
   <si>
-    <t>ninja</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -60,9 +51,6 @@
     <t>kempo</t>
   </si>
   <si>
-    <t>lala</t>
-  </si>
-  <si>
     <t>juan</t>
   </si>
   <si>
@@ -73,6 +61,39 @@
   </si>
   <si>
     <t>id_habilidad</t>
+  </si>
+  <si>
+    <t>dojos</t>
+  </si>
+  <si>
+    <t>ubicaciónes</t>
+  </si>
+  <si>
+    <t>ninjas</t>
+  </si>
+  <si>
+    <t>habilidades</t>
+  </si>
+  <si>
+    <t>habilidades_ninjas</t>
+  </si>
+  <si>
+    <t>defender</t>
+  </si>
+  <si>
+    <t>atacar</t>
+  </si>
+  <si>
+    <t>id_ninja</t>
+  </si>
+  <si>
+    <t>rosas</t>
+  </si>
+  <si>
+    <t>gory</t>
+  </si>
+  <si>
+    <t>ciruelos</t>
   </si>
 </sst>
 </file>
@@ -88,12 +109,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,8 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,63 +459,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB1D070-0521-48AA-8BCB-E4ED56EE80DA}">
-  <dimension ref="B3:M13"/>
+  <dimension ref="B3:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -489,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -498,48 +533,126 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>33</v>
+      </c>
       <c r="J6">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F12" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>